<commit_message>
Results including R11 CZ data
</commit_message>
<xml_diff>
--- a/tables/tab_weight_sums.xlsx
+++ b/tables/tab_weight_sums.xlsx
@@ -3320,25 +3320,25 @@
         <v>45</v>
       </c>
       <c r="B110" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C110" t="n">
-        <v>2420</v>
+        <v>1805</v>
       </c>
       <c r="D110" t="n">
-        <v>2419.99993860722</v>
+        <v>1805.00001305901</v>
       </c>
       <c r="E110" t="n">
-        <v>2419.99996938556</v>
+        <v>1804.9999993369</v>
       </c>
       <c r="F110" t="n">
-        <v>72429867.4458265</v>
+        <v>9081752.44566366</v>
       </c>
       <c r="G110" t="n">
-        <v>0.0000613927841186523</v>
+        <v>0.0000130590051412582</v>
       </c>
       <c r="H110" t="n">
-        <v>0.00003061443567276</v>
+        <v>0.000000663101673126221</v>
       </c>
     </row>
     <row r="111">
@@ -3346,25 +3346,25 @@
         <v>45</v>
       </c>
       <c r="B111" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C111" t="n">
-        <v>1844</v>
+        <v>2420</v>
       </c>
       <c r="D111" t="n">
-        <v>1844.00003373623</v>
+        <v>2419.99993860722</v>
       </c>
       <c r="E111" t="n">
-        <v>1843.99996042252</v>
+        <v>2419.99996938556</v>
       </c>
       <c r="F111" t="n">
-        <v>41548145.1189518</v>
+        <v>72429867.4458265</v>
       </c>
       <c r="G111" t="n">
-        <v>0.0000337362289428711</v>
+        <v>0.0000613927841186523</v>
       </c>
       <c r="H111" t="n">
-        <v>0.0000395774841308594</v>
+        <v>0.00003061443567276</v>
       </c>
     </row>
     <row r="112">
@@ -3372,25 +3372,25 @@
         <v>45</v>
       </c>
       <c r="B112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C112" t="n">
-        <v>1563</v>
+        <v>1844</v>
       </c>
       <c r="D112" t="n">
-        <v>1563</v>
+        <v>1844.00003373623</v>
       </c>
       <c r="E112" t="n">
-        <v>1562.99999660254</v>
+        <v>1843.99996042252</v>
       </c>
       <c r="F112" t="n">
-        <v>4723642.00651646</v>
+        <v>41548145.1189518</v>
       </c>
       <c r="G112" t="n">
-        <v>0</v>
+        <v>0.0000337362289428711</v>
       </c>
       <c r="H112" t="n">
-        <v>0.00000339746475219727</v>
+        <v>0.0000395774841308594</v>
       </c>
     </row>
     <row r="113">
@@ -3398,25 +3398,25 @@
         <v>45</v>
       </c>
       <c r="B113" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C113" t="n">
-        <v>1771</v>
+        <v>1563</v>
       </c>
       <c r="D113" t="n">
-        <v>1770.98797518015</v>
+        <v>1563</v>
       </c>
       <c r="E113" t="n">
-        <v>1770.99999552965</v>
+        <v>1562.99999660254</v>
       </c>
       <c r="F113" t="n">
-        <v>56395314.7733212</v>
+        <v>4723642.00651646</v>
       </c>
       <c r="G113" t="n">
-        <v>0.0120248198509216</v>
+        <v>0</v>
       </c>
       <c r="H113" t="n">
-        <v>0.0000044703483581543</v>
+        <v>0.00000339746475219727</v>
       </c>
     </row>
     <row r="114">
@@ -3424,25 +3424,25 @@
         <v>45</v>
       </c>
       <c r="B114" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C114" t="n">
-        <v>1684</v>
+        <v>1771</v>
       </c>
       <c r="D114" t="n">
-        <v>1683.99995458126</v>
+        <v>1770.98797518015</v>
       </c>
       <c r="E114" t="n">
-        <v>1684.00000494719</v>
+        <v>1770.99999552965</v>
       </c>
       <c r="F114" t="n">
-        <v>55980686.1269474</v>
+        <v>56395314.7733212</v>
       </c>
       <c r="G114" t="n">
-        <v>0.0000454187393188477</v>
+        <v>0.0120248198509216</v>
       </c>
       <c r="H114" t="n">
-        <v>0.00000494718551635742</v>
+        <v>0.0000044703483581543</v>
       </c>
     </row>
     <row r="115">
@@ -3450,25 +3450,25 @@
         <v>45</v>
       </c>
       <c r="B115" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C115" t="n">
-        <v>2757</v>
+        <v>1684</v>
       </c>
       <c r="D115" t="n">
-        <v>2757.00006876886</v>
+        <v>1683.99995458126</v>
       </c>
       <c r="E115" t="n">
-        <v>2757.00000843406</v>
+        <v>1684.00000494719</v>
       </c>
       <c r="F115" t="n">
-        <v>9022623.00599366</v>
+        <v>55980686.1269474</v>
       </c>
       <c r="G115" t="n">
-        <v>0.0000687688589096069</v>
+        <v>0.0000454187393188477</v>
       </c>
       <c r="H115" t="n">
-        <v>0.00000843405723571777</v>
+        <v>0.00000494718551635742</v>
       </c>
     </row>
     <row r="116">
@@ -3476,25 +3476,25 @@
         <v>45</v>
       </c>
       <c r="B116" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C116" t="n">
-        <v>1563</v>
+        <v>2757</v>
       </c>
       <c r="D116" t="n">
-        <v>1562.99998825788</v>
+        <v>2757.00006876886</v>
       </c>
       <c r="E116" t="n">
-        <v>1563.00000974536</v>
+        <v>2757.00000843406</v>
       </c>
       <c r="F116" t="n">
-        <v>3302096.02832794</v>
+        <v>9022623.00599366</v>
       </c>
       <c r="G116" t="n">
-        <v>0.000011742115020752</v>
+        <v>0.0000687688589096069</v>
       </c>
       <c r="H116" t="n">
-        <v>0.00000974535942077637</v>
+        <v>0.00000843405723571777</v>
       </c>
     </row>
     <row r="117">
@@ -3502,25 +3502,25 @@
         <v>45</v>
       </c>
       <c r="B117" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C117" t="n">
-        <v>2118</v>
+        <v>1563</v>
       </c>
       <c r="D117" t="n">
-        <v>2117.99999642372</v>
+        <v>1562.99998825788</v>
       </c>
       <c r="E117" t="n">
-        <v>2117.99999937415</v>
+        <v>1563.00000974536</v>
       </c>
       <c r="F117" t="n">
-        <v>8206689.0154779</v>
+        <v>3302096.02832794</v>
       </c>
       <c r="G117" t="n">
-        <v>0.00000357627868652344</v>
+        <v>0.000011742115020752</v>
       </c>
       <c r="H117" t="n">
-        <v>0.000000625848770141602</v>
+        <v>0.00000974535942077637</v>
       </c>
     </row>
     <row r="118">
@@ -3528,25 +3528,25 @@
         <v>45</v>
       </c>
       <c r="B118" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C118" t="n">
-        <v>2017</v>
+        <v>2118</v>
       </c>
       <c r="D118" t="n">
-        <v>2016.99999380112</v>
+        <v>2117.99999642372</v>
       </c>
       <c r="E118" t="n">
-        <v>2017.00000298023</v>
+        <v>2117.99999937415</v>
       </c>
       <c r="F118" t="n">
-        <v>4251953.9770484</v>
+        <v>8206689.0154779</v>
       </c>
       <c r="G118" t="n">
-        <v>0.00000619888305664062</v>
+        <v>0.00000357627868652344</v>
       </c>
       <c r="H118" t="n">
-        <v>0.00000298023223876953</v>
+        <v>0.000000625848770141602</v>
       </c>
     </row>
     <row r="119">
@@ -3554,25 +3554,25 @@
         <v>45</v>
       </c>
       <c r="B119" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C119" t="n">
-        <v>842</v>
+        <v>2017</v>
       </c>
       <c r="D119" t="n">
-        <v>841.999966621399</v>
+        <v>2016.99999380112</v>
       </c>
       <c r="E119" t="n">
-        <v>841.999996364117</v>
+        <v>2017.00000298023</v>
       </c>
       <c r="F119" t="n">
-        <v>317250.997549854</v>
+        <v>4251953.9770484</v>
       </c>
       <c r="G119" t="n">
-        <v>0.0000333786010742188</v>
+        <v>0.00000619888305664062</v>
       </c>
       <c r="H119" t="n">
-        <v>0.00000363588333129883</v>
+        <v>0.00000298023223876953</v>
       </c>
     </row>
     <row r="120">
@@ -3580,25 +3580,25 @@
         <v>45</v>
       </c>
       <c r="B120" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C120" t="n">
-        <v>2865</v>
+        <v>842</v>
       </c>
       <c r="D120" t="n">
-        <v>2870.72513353825</v>
+        <v>841.999966621399</v>
       </c>
       <c r="E120" t="n">
-        <v>2865.00003999472</v>
+        <v>841.999996364117</v>
       </c>
       <c r="F120" t="n">
-        <v>51653102.7579308</v>
+        <v>317250.997549854</v>
       </c>
       <c r="G120" t="n">
-        <v>5.72513353824615</v>
+        <v>0.0000333786010742188</v>
       </c>
       <c r="H120" t="n">
-        <v>0.0000399947166442871</v>
+        <v>0.00000363588333129883</v>
       </c>
     </row>
     <row r="121">
@@ -3606,25 +3606,25 @@
         <v>45</v>
       </c>
       <c r="B121" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C121" t="n">
-        <v>1365</v>
+        <v>2865</v>
       </c>
       <c r="D121" t="n">
-        <v>1365.00001290441</v>
+        <v>2870.72513353825</v>
       </c>
       <c r="E121" t="n">
-        <v>1364.9999961406</v>
+        <v>2865.00003999472</v>
       </c>
       <c r="F121" t="n">
-        <v>2430151.99910849</v>
+        <v>51653102.7579308</v>
       </c>
       <c r="G121" t="n">
-        <v>0.0000129044055938721</v>
+        <v>5.72513353824615</v>
       </c>
       <c r="H121" t="n">
-        <v>0.00000385940074920654</v>
+        <v>0.0000399947166442871</v>
       </c>
     </row>
     <row r="122">
@@ -3632,25 +3632,25 @@
         <v>45</v>
       </c>
       <c r="B122" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C122" t="n">
-        <v>1695</v>
+        <v>1365</v>
       </c>
       <c r="D122" t="n">
-        <v>1695.00000739098</v>
+        <v>1365.00001290441</v>
       </c>
       <c r="E122" t="n">
-        <v>1694.99996978045</v>
+        <v>1364.9999961406</v>
       </c>
       <c r="F122" t="n">
-        <v>15083913.783133</v>
+        <v>2430151.99910849</v>
       </c>
       <c r="G122" t="n">
-        <v>0.00000739097595214844</v>
+        <v>0.0000129044055938721</v>
       </c>
       <c r="H122" t="n">
-        <v>0.000030219554901123</v>
+        <v>0.00000385940074920654</v>
       </c>
     </row>
     <row r="123">
@@ -3658,25 +3658,25 @@
         <v>45</v>
       </c>
       <c r="B123" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C123" t="n">
-        <v>1337</v>
+        <v>1695</v>
       </c>
       <c r="D123" t="n">
-        <v>1336.99999719858</v>
+        <v>1695.00000739098</v>
       </c>
       <c r="E123" t="n">
-        <v>1337.00000631809</v>
+        <v>1694.99996978045</v>
       </c>
       <c r="F123" t="n">
-        <v>4572917.03000665</v>
+        <v>15083913.783133</v>
       </c>
       <c r="G123" t="n">
-        <v>0.00000280141830444336</v>
+        <v>0.00000739097595214844</v>
       </c>
       <c r="H123" t="n">
-        <v>0.00000631809234619141</v>
+        <v>0.000030219554901123</v>
       </c>
     </row>
     <row r="124">
@@ -3684,25 +3684,25 @@
         <v>45</v>
       </c>
       <c r="B124" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C124" t="n">
-        <v>1442</v>
+        <v>1337</v>
       </c>
       <c r="D124" t="n">
-        <v>1441.99996781349</v>
+        <v>1336.99999719858</v>
       </c>
       <c r="E124" t="n">
-        <v>1442.00000235438</v>
+        <v>1337.00000631809</v>
       </c>
       <c r="F124" t="n">
-        <v>31085397.0146179</v>
+        <v>4572917.03000665</v>
       </c>
       <c r="G124" t="n">
-        <v>0.0000321865081787109</v>
+        <v>0.00000280141830444336</v>
       </c>
       <c r="H124" t="n">
-        <v>0.00000235438346862793</v>
+        <v>0.00000631809234619141</v>
       </c>
     </row>
     <row r="125">
@@ -3710,25 +3710,25 @@
         <v>45</v>
       </c>
       <c r="B125" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C125" t="n">
-        <v>1373</v>
+        <v>1442</v>
       </c>
       <c r="D125" t="n">
-        <v>1373.00000321865</v>
+        <v>1441.99996781349</v>
       </c>
       <c r="E125" t="n">
-        <v>1373.00000679493</v>
+        <v>1442.00000235438</v>
       </c>
       <c r="F125" t="n">
-        <v>9116355.00341654</v>
+        <v>31085397.0146179</v>
       </c>
       <c r="G125" t="n">
-        <v>0.00000321865081787109</v>
+        <v>0.0000321865081787109</v>
       </c>
       <c r="H125" t="n">
-        <v>0.00000679492950439453</v>
+        <v>0.00000235438346862793</v>
       </c>
     </row>
     <row r="126">
@@ -3736,25 +3736,25 @@
         <v>45</v>
       </c>
       <c r="B126" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C126" t="n">
-        <v>1563</v>
+        <v>1373</v>
       </c>
       <c r="D126" t="n">
-        <v>1563.00002384186</v>
+        <v>1373.00000321865</v>
       </c>
       <c r="E126" t="n">
-        <v>1563.0000128448</v>
+        <v>1373.00000679493</v>
       </c>
       <c r="F126" t="n">
-        <v>5682811.0575676</v>
+        <v>9116355.00341654</v>
       </c>
       <c r="G126" t="n">
-        <v>0.0000238418579101562</v>
+        <v>0.00000321865081787109</v>
       </c>
       <c r="H126" t="n">
-        <v>0.0000128448009490967</v>
+        <v>0.00000679492950439453</v>
       </c>
     </row>
     <row r="127">
@@ -3762,25 +3762,25 @@
         <v>45</v>
       </c>
       <c r="B127" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C127" t="n">
-        <v>1230</v>
+        <v>1563</v>
       </c>
       <c r="D127" t="n">
-        <v>1229.99998766184</v>
+        <v>1563.00002384186</v>
       </c>
       <c r="E127" t="n">
-        <v>1230.00000306964</v>
+        <v>1563.0000128448</v>
       </c>
       <c r="F127" t="n">
-        <v>8692463.0048871</v>
+        <v>5682811.0575676</v>
       </c>
       <c r="G127" t="n">
-        <v>0.0000123381614685059</v>
+        <v>0.0000238418579101562</v>
       </c>
       <c r="H127" t="n">
-        <v>0.00000306963920593262</v>
+        <v>0.0000128448009490967</v>
       </c>
     </row>
     <row r="128">
@@ -3788,25 +3788,25 @@
         <v>45</v>
       </c>
       <c r="B128" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C128" t="n">
-        <v>1248</v>
+        <v>1230</v>
       </c>
       <c r="D128" t="n">
-        <v>1248</v>
+        <v>1229.99998766184</v>
       </c>
       <c r="E128" t="n">
-        <v>1248.00000017881</v>
+        <v>1230.00000306964</v>
       </c>
       <c r="F128" t="n">
-        <v>1799440.98971784</v>
+        <v>8692463.0048871</v>
       </c>
       <c r="G128" t="n">
-        <v>0</v>
+        <v>0.0000123381614685059</v>
       </c>
       <c r="H128" t="n">
-        <v>0.000000178813934326172</v>
+        <v>0.00000306963920593262</v>
       </c>
     </row>
     <row r="129">
@@ -3814,24 +3814,50 @@
         <v>45</v>
       </c>
       <c r="B129" t="s">
+        <v>29</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1248</v>
+      </c>
+      <c r="D129" t="n">
+        <v>1248</v>
+      </c>
+      <c r="E129" t="n">
+        <v>1248.00000017881</v>
+      </c>
+      <c r="F129" t="n">
+        <v>1799440.98971784</v>
+      </c>
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" t="n">
+        <v>0.000000178813934326172</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>45</v>
+      </c>
+      <c r="B130" t="s">
         <v>41</v>
       </c>
-      <c r="C129" t="n">
+      <c r="C130" t="n">
         <v>1442</v>
       </c>
-      <c r="D129" t="n">
+      <c r="D130" t="n">
         <v>1442.00000609457</v>
       </c>
-      <c r="E129" t="n">
+      <c r="E130" t="n">
         <v>1441.99999478087</v>
       </c>
-      <c r="F129" t="n">
+      <c r="F130" t="n">
         <v>4555339.98873085</v>
       </c>
-      <c r="G129" t="n">
+      <c r="G130" t="n">
         <v>0.00000609457492828369</v>
       </c>
-      <c r="H129" t="n">
+      <c r="H130" t="n">
         <v>0.00000521913170814514</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CZ Version notes edition 2.0 (published 06.01.2025):
Changes from edition 1.0:

Weights recalculated.
For IDNOs 79569 and 59611: Value on variable IDNO was missing in edition 1.0. This has been corrected.
IDNO 104814: Respondent younger than ESS target population (calculated age 14 when questionnaire completed). Values were set to missing in edition 1.0 but have been included in edition 2.0.
Variables mbrn, mbrn2-9 have been removed.
</commit_message>
<xml_diff>
--- a/tables/tab_weight_sums.xlsx
+++ b/tables/tab_weight_sums.xlsx
@@ -3326,19 +3326,19 @@
         <v>1805</v>
       </c>
       <c r="D110" t="n">
-        <v>1805.00001305901</v>
+        <v>1805.0000166595</v>
       </c>
       <c r="E110" t="n">
-        <v>1804.9999993369</v>
+        <v>1804.99993595481</v>
       </c>
       <c r="F110" t="n">
-        <v>9081752.44566366</v>
+        <v>9081752.12676029</v>
       </c>
       <c r="G110" t="n">
-        <v>0.0000130590051412582</v>
+        <v>0.0000166594982147217</v>
       </c>
       <c r="H110" t="n">
-        <v>0.000000663101673126221</v>
+        <v>0.0000640451908111572</v>
       </c>
     </row>
     <row r="111">

</xml_diff>

<commit_message>
R11 CZ new data
</commit_message>
<xml_diff>
--- a/tables/tab_weight_sums.xlsx
+++ b/tables/tab_weight_sums.xlsx
@@ -527,10 +527,10 @@
         <v>7288046.9571054</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00000464916229248047</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00000202655792236328</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00000774860382080078</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00000709295272827148</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -605,10 +605,10 @@
         <v>8934963.84038706</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00000462611205875874</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.000000886386260390282</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -631,10 +631,10 @@
         <v>70160637.5944614</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000105142593383789</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00000282377004623413</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00000295042991638184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0000113844871520996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00000596046447753906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.00000369548797607422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -761,10 +761,10 @@
         <v>53613538.7013853</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00000733137130737305</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00000371038913726807</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -787,10 +787,10 @@
         <v>52974790.8216715</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0000103116035461426</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0000063478946685791</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00000208616256713867</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -839,10 +839,10 @@
         <v>3592163.13079</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0000185072422027588</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.00000867247581481934</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -865,10 +865,10 @@
         <v>5895900.09983629</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0000031888484954834</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00000157207250595093</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -891,10 +891,10 @@
         <v>2513384.07920673</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00000858306884765625</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00000649690628051758</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -917,10 +917,10 @@
         <v>13979215.1346058</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0000860691070556641</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0.00000141561031341553</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -943,10 +943,10 @@
         <v>4177168.94835234</v>
       </c>
       <c r="G18" t="n">
-        <v>0.000056922435760498</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0.00000515580177307129</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -969,10 +969,10 @@
         <v>36325274.7929096</v>
       </c>
       <c r="G19" t="n">
-        <v>0.00000649690628051758</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0.00000160932540893555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -995,10 +995,10 @@
         <v>6975473.98638679</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00000517908483743668</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0.00000208849087357521</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1024,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0.00000140070915222168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>0.00000250339508056641</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1073,10 +1073,10 @@
         <v>7444897.09973335</v>
       </c>
       <c r="G23" t="n">
-        <v>0.000000268220901489258</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0000130832195281982</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1099,10 +1099,10 @@
         <v>9389774.89709854</v>
       </c>
       <c r="G24" t="n">
-        <v>0.00000512599945068359</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>0.000000119209289550781</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00000368058681488037</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1151,10 +1151,10 @@
         <v>8930127.15063989</v>
       </c>
       <c r="G26" t="n">
-        <v>0.000255435705184937</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0000108126550912857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1177,10 +1177,10 @@
         <v>71294560.3376627</v>
       </c>
       <c r="G27" t="n">
-        <v>0.000112593173980713</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>0.00000676512718200684</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1203,10 +1203,10 @@
         <v>1104499.03078377</v>
       </c>
       <c r="G28" t="n">
-        <v>0.000053107738494873</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0000238418579101562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1229,10 +1229,10 @@
         <v>39414698.9142895</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0000109672546386719</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0000012516975402832</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1258,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0000241398811340332</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1281,10 +1281,10 @@
         <v>54431181.4528704</v>
       </c>
       <c r="G31" t="n">
-        <v>0.00000345706939697266</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0000102519989013672</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1307,10 +1307,10 @@
         <v>53795163.6177301</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0000182390213012695</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0.00000232458114624023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1333,10 +1333,10 @@
         <v>8406037.17103601</v>
       </c>
       <c r="G33" t="n">
-        <v>0.000161647796630859</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0000216066837310791</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1359,10 +1359,10 @@
         <v>3687781.80673718</v>
       </c>
       <c r="G34" t="n">
-        <v>0.000509142875671387</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0000223219394683838</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1385,10 +1385,10 @@
         <v>6130399.86485615</v>
       </c>
       <c r="G35" t="n">
-        <v>0.00000219047069549561</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>0.00001554936170578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1411,10 +1411,10 @@
         <v>265989.013370126</v>
       </c>
       <c r="G36" t="n">
-        <v>0.00000792741775512695</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0.000010073184967041</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1437,10 +1437,10 @@
         <v>52383691.6470528</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0000224709510803223</v>
+        <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0.00000154972076416016</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1463,10 +1463,10 @@
         <v>2464810.96848845</v>
       </c>
       <c r="G38" t="n">
-        <v>0.00104199349880219</v>
+        <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>0.00000110268592834473</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1489,10 +1489,10 @@
         <v>14179347.5006521</v>
       </c>
       <c r="G39" t="n">
-        <v>0.0000628232955932617</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>0.00000163912773132324</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1515,10 +1515,10 @@
         <v>4277120.93010545</v>
       </c>
       <c r="G40" t="n">
-        <v>0.00000822544097900391</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>0.00000280141830444336</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1541,10 +1541,10 @@
         <v>32258355.1955223</v>
       </c>
       <c r="G41" t="n">
-        <v>0.00000619888305664062</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0000101923942565918</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1567,10 +1567,10 @@
         <v>8880498.30265343</v>
       </c>
       <c r="G42" t="n">
-        <v>0.000634707510471344</v>
+        <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>0.00000818260014057159</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1593,10 +1593,10 @@
         <v>121153926.161826</v>
       </c>
       <c r="G43" t="n">
-        <v>0.00000810623168945312</v>
+        <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>0.00000370293855667114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1619,10 +1619,10 @@
         <v>8133873.55148792</v>
       </c>
       <c r="G44" t="n">
-        <v>0.00000137090682983398</v>
+        <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0000447779893875122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1648,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>0.0000190138816833496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1671,10 +1671,10 @@
         <v>7549265.33127204</v>
       </c>
       <c r="G46" t="n">
-        <v>0.00000682473182678223</v>
+        <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>0.00000671297311782837</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1697,10 +1697,10 @@
         <v>9464647.24227786</v>
       </c>
       <c r="G47" t="n">
-        <v>0.00000411272048950195</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>0.00000762939453125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1723,10 +1723,10 @@
         <v>6045658.27611834</v>
       </c>
       <c r="G48" t="n">
-        <v>0.00000360608100891113</v>
+        <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>0.00000161677598953247</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>0.00000524520874023438</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1775,10 +1775,10 @@
         <v>723947.003912181</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0000057220458984375</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>0.00000044703483581543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1801,10 +1801,10 @@
         <v>8939378.03305686</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0000554323196411133</v>
+        <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>0.0000266432762145996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1827,10 +1827,10 @@
         <v>71620594.2285061</v>
       </c>
       <c r="G52" t="n">
-        <v>0.0000178813934326172</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>0.0000153183937072754</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>0.0000112056732177734</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1879,10 +1879,10 @@
         <v>1103907.01370314</v>
       </c>
       <c r="G54" t="n">
-        <v>0.0000219345092773438</v>
+        <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>0.00000619888305664062</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1905,10 +1905,10 @@
         <v>39679882.1473122</v>
       </c>
       <c r="G55" t="n">
-        <v>0.000000536441802978516</v>
+        <v>0</v>
       </c>
       <c r="H55" t="n">
-        <v>0.00000810623168945312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1934,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>0.0000222921371459961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1957,10 +1957,10 @@
         <v>54806402.7631283</v>
       </c>
       <c r="G57" t="n">
-        <v>0.0000141263008117676</v>
+        <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>0.00000721216201782227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1983,10 +1983,10 @@
         <v>54402028.8443565</v>
       </c>
       <c r="G58" t="n">
-        <v>0.0000147223472595215</v>
+        <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>0.0000240802764892578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2009,10 +2009,10 @@
         <v>3511099.92107376</v>
       </c>
       <c r="G59" t="n">
-        <v>0.0318195670843124</v>
+        <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>0.00000258535146713257</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2035,10 +2035,10 @@
         <v>8356454.90512252</v>
       </c>
       <c r="G60" t="n">
-        <v>0.0612244009971619</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
-        <v>0.0000167787075042725</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2061,10 +2061,10 @@
         <v>3823943.96580756</v>
       </c>
       <c r="G61" t="n">
-        <v>0.0000126361846923828</v>
+        <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>0.00000461935997009277</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2087,10 +2087,10 @@
         <v>281042.997706681</v>
       </c>
       <c r="G62" t="n">
-        <v>0.00000810623168945312</v>
+        <v>0</v>
       </c>
       <c r="H62" t="n">
-        <v>0.0000056922435760498</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2113,10 +2113,10 @@
         <v>52403798.7792492</v>
       </c>
       <c r="G63" t="n">
-        <v>0.0899392366409302</v>
+        <v>0</v>
       </c>
       <c r="H63" t="n">
-        <v>0.0000194013118743896</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2139,10 +2139,10 @@
         <v>2387464.00121599</v>
       </c>
       <c r="G64" t="n">
-        <v>0.00000033155083656311</v>
+        <v>0</v>
       </c>
       <c r="H64" t="n">
-        <v>0.00000254437327384949</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2165,10 +2165,10 @@
         <v>1629088.00758421</v>
       </c>
       <c r="G65" t="n">
-        <v>0.0000101923942565918</v>
+        <v>0</v>
       </c>
       <c r="H65" t="n">
-        <v>0.00000780820846557617</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2191,10 +2191,10 @@
         <v>509929.003072903</v>
       </c>
       <c r="G66" t="n">
-        <v>0.00000452995300292969</v>
+        <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>0.0000315755605697632</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2217,10 +2217,10 @@
         <v>14418459.8278999</v>
       </c>
       <c r="G67" t="n">
-        <v>0.0000105500221252441</v>
+        <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>0.0000151991844177246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2243,10 +2243,10 @@
         <v>4356685.12016535</v>
       </c>
       <c r="G68" t="n">
-        <v>0.000003814697265625</v>
+        <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>0.000000596046447753906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2269,10 +2269,10 @@
         <v>32189898.5731602</v>
       </c>
       <c r="G69" t="n">
-        <v>0.00000292062759399414</v>
+        <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>0.0000044703483581543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2295,10 +2295,10 @@
         <v>8867130.94368577</v>
       </c>
       <c r="G70" t="n">
-        <v>0.0161583125591278</v>
+        <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>0.0000012814998626709</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2321,10 +2321,10 @@
         <v>5996452.96997856</v>
       </c>
       <c r="G71" t="n">
-        <v>0.0000119246542453766</v>
+        <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>0.0000113397836685181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2350,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>0.00000736117362976074</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>0.00000417232513427734</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2399,10 +2399,10 @@
         <v>4593419.17261481</v>
       </c>
       <c r="G74" t="n">
-        <v>0.0442112982273102</v>
+        <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>0.00000226497650146484</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2425,10 +2425,10 @@
         <v>7647176.04532838</v>
       </c>
       <c r="G75" t="n">
-        <v>0.00000312924385070801</v>
+        <v>0</v>
       </c>
       <c r="H75" t="n">
-        <v>0.0000180453062057495</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2451,10 +2451,10 @@
         <v>9629391.00146294</v>
       </c>
       <c r="G76" t="n">
-        <v>0.00000292062759399414</v>
+        <v>0</v>
       </c>
       <c r="H76" t="n">
-        <v>0.00000110268592834473</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2477,10 +2477,10 @@
         <v>5917533.95172767</v>
       </c>
       <c r="G77" t="n">
-        <v>0.00000904500484466553</v>
+        <v>0</v>
       </c>
       <c r="H77" t="n">
-        <v>0.0000234246253967285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>0.000000774860382080078</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2529,10 +2529,10 @@
         <v>752304.001590237</v>
       </c>
       <c r="G79" t="n">
-        <v>0.00000800192356109619</v>
+        <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>0.00000282377004623413</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2555,10 +2555,10 @@
         <v>8982035.99534929</v>
       </c>
       <c r="G80" t="n">
-        <v>0.000030815601348877</v>
+        <v>0</v>
       </c>
       <c r="H80" t="n">
-        <v>0.0000127255916595459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2581,10 +2581,10 @@
         <v>71677231.1322391</v>
       </c>
       <c r="G81" t="n">
-        <v>0.000496506690979004</v>
+        <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>0.0000182688236236572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2607,10 +2607,10 @@
         <v>1111597.01883793</v>
       </c>
       <c r="G82" t="n">
-        <v>0.00000578165054321289</v>
+        <v>0</v>
       </c>
       <c r="H82" t="n">
-        <v>0.00000143051147460938</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2633,10 +2633,10 @@
         <v>40639381.0653687</v>
       </c>
       <c r="G83" t="n">
-        <v>0.0000149011611938477</v>
+        <v>0</v>
       </c>
       <c r="H83" t="n">
-        <v>0.00000485777854919434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2662,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="H84" t="n">
-        <v>0.00000423192977905273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2685,10 +2685,10 @@
         <v>55700113.7375832</v>
       </c>
       <c r="G85" t="n">
-        <v>0.000000357627868652344</v>
+        <v>0</v>
       </c>
       <c r="H85" t="n">
-        <v>0.00000751018524169922</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2711,10 +2711,10 @@
         <v>55085594.2070484</v>
       </c>
       <c r="G86" t="n">
-        <v>0.000027775764465332</v>
+        <v>0</v>
       </c>
       <c r="H86" t="n">
-        <v>0.00000593066215515137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2737,10 +2737,10 @@
         <v>9167895.95185779</v>
       </c>
       <c r="G87" t="n">
-        <v>0.000102415680885315</v>
+        <v>0</v>
       </c>
       <c r="H87" t="n">
-        <v>0.00000443309545516968</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2763,10 +2763,10 @@
         <v>3461468.02611649</v>
       </c>
       <c r="G88" t="n">
-        <v>0.0000782608985900879</v>
+        <v>0</v>
       </c>
       <c r="H88" t="n">
-        <v>0.00000751018524169922</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -2789,10 +2789,10 @@
         <v>8313539.01728988</v>
       </c>
       <c r="G89" t="n">
-        <v>0.0000588297843933105</v>
+        <v>0</v>
       </c>
       <c r="H89" t="n">
-        <v>0.00000324845314025879</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -2815,10 +2815,10 @@
         <v>4005909.01520103</v>
       </c>
       <c r="G90" t="n">
-        <v>0.00000141561031341553</v>
+        <v>0</v>
       </c>
       <c r="H90" t="n">
-        <v>0.00000877678394317627</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2841,10 +2841,10 @@
         <v>6629200.03104955</v>
       </c>
       <c r="G91" t="n">
-        <v>0.0000392645597457886</v>
+        <v>0</v>
       </c>
       <c r="H91" t="n">
-        <v>0.0000135749578475952</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2867,10 +2867,10 @@
         <v>299803.000455722</v>
       </c>
       <c r="G92" t="n">
-        <v>0.0000380873680114746</v>
+        <v>0</v>
       </c>
       <c r="H92" t="n">
-        <v>0.00000301003456115723</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2893,10 +2893,10 @@
         <v>51599668.2816744</v>
       </c>
       <c r="G93" t="n">
-        <v>0.0000142455101013184</v>
+        <v>0</v>
       </c>
       <c r="H93" t="n">
-        <v>0.0000183582305908203</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2919,10 +2919,10 @@
         <v>2373311.98749132</v>
       </c>
       <c r="G94" t="n">
-        <v>0.0000174343585968018</v>
+        <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>0.00000941753387451172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2945,10 +2945,10 @@
         <v>1590244.98492479</v>
       </c>
       <c r="G95" t="n">
-        <v>0.000012516975402832</v>
+        <v>0</v>
       </c>
       <c r="H95" t="n">
-        <v>0.00000923871994018555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -2971,10 +2971,10 @@
         <v>509572.005320806</v>
       </c>
       <c r="G96" t="n">
-        <v>0.000047832727432251</v>
+        <v>0</v>
       </c>
       <c r="H96" t="n">
-        <v>0.0000264719128608704</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2997,10 +2997,10 @@
         <v>1735434.99294203</v>
       </c>
       <c r="G97" t="n">
-        <v>0.0000430494546890259</v>
+        <v>0</v>
       </c>
       <c r="H97" t="n">
-        <v>0.0000140368938446045</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -3023,10 +3023,10 @@
         <v>14763684.014678</v>
       </c>
       <c r="G98" t="n">
-        <v>0.0000175237655639648</v>
+        <v>0</v>
       </c>
       <c r="H98" t="n">
-        <v>0.00000241398811340332</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -3049,10 +3049,10 @@
         <v>4469778.0367732</v>
       </c>
       <c r="G99" t="n">
-        <v>0.0000299215316772461</v>
+        <v>0</v>
       </c>
       <c r="H99" t="n">
-        <v>0.00000593066215515137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3075,10 +3075,10 @@
         <v>31982941.3473606</v>
       </c>
       <c r="G100" t="n">
-        <v>0.0000866055488586426</v>
+        <v>0</v>
       </c>
       <c r="H100" t="n">
-        <v>0.0000233650207519531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -3101,10 +3101,10 @@
         <v>8915623.85886908</v>
       </c>
       <c r="G101" t="n">
-        <v>0.0000110864639282227</v>
+        <v>0</v>
       </c>
       <c r="H101" t="n">
-        <v>0.0000317096710205078</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -3127,10 +3127,10 @@
         <v>5891214.91828933</v>
       </c>
       <c r="G102" t="n">
-        <v>0.0000337362289428711</v>
+        <v>0</v>
       </c>
       <c r="H102" t="n">
-        <v>0.0000156238675117493</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -3156,7 +3156,7 @@
         <v>0</v>
       </c>
       <c r="H103" t="n">
-        <v>0.00000703334808349609</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -3182,7 +3182,7 @@
         <v>0</v>
       </c>
       <c r="H104" t="n">
-        <v>0.00000858306884765625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -3205,10 +3205,10 @@
         <v>4591487.01416329</v>
       </c>
       <c r="G105" t="n">
-        <v>0.00000599771738052368</v>
+        <v>0</v>
       </c>
       <c r="H105" t="n">
-        <v>0.00000173225998878479</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -3231,10 +3231,10 @@
         <v>7789727.9292345</v>
       </c>
       <c r="G106" t="n">
-        <v>0.0000445246696472168</v>
+        <v>0</v>
       </c>
       <c r="H106" t="n">
-        <v>0.0000137835741043091</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -3257,10 +3257,10 @@
         <v>9804276.02618933</v>
       </c>
       <c r="G107" t="n">
-        <v>0.0000991225242614746</v>
+        <v>0</v>
       </c>
       <c r="H107" t="n">
-        <v>0.000000804662704467773</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -3286,7 +3286,7 @@
         <v>0</v>
       </c>
       <c r="H108" t="n">
-        <v>0.0000118613243103027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -3309,10 +3309,10 @@
         <v>772474.000267684</v>
       </c>
       <c r="G109" t="n">
-        <v>0.0000180304050445557</v>
+        <v>0</v>
       </c>
       <c r="H109" t="n">
-        <v>0.00000154972076416016</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -3332,13 +3332,13 @@
         <v>1804.99993595481</v>
       </c>
       <c r="F110" t="n">
-        <v>9081752.12676029</v>
+        <v>9081752.12676031</v>
       </c>
       <c r="G110" t="n">
-        <v>0.0000166594982147217</v>
+        <v>0</v>
       </c>
       <c r="H110" t="n">
-        <v>0.0000640451908111572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -3361,10 +3361,10 @@
         <v>72429867.4458265</v>
       </c>
       <c r="G111" t="n">
-        <v>0.0000613927841186523</v>
+        <v>0</v>
       </c>
       <c r="H111" t="n">
-        <v>0.00003061443567276</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -3387,10 +3387,10 @@
         <v>41548145.1189518</v>
       </c>
       <c r="G112" t="n">
-        <v>0.0000337362289428711</v>
+        <v>0</v>
       </c>
       <c r="H112" t="n">
-        <v>0.0000395774841308594</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="H113" t="n">
-        <v>0.00000339746475219727</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -3439,10 +3439,10 @@
         <v>56395314.7733212</v>
       </c>
       <c r="G114" t="n">
-        <v>0.0120248198509216</v>
+        <v>0</v>
       </c>
       <c r="H114" t="n">
-        <v>0.0000044703483581543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -3465,10 +3465,10 @@
         <v>55980686.1269474</v>
       </c>
       <c r="G115" t="n">
-        <v>0.0000454187393188477</v>
+        <v>0</v>
       </c>
       <c r="H115" t="n">
-        <v>0.00000494718551635742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -3491,10 +3491,10 @@
         <v>9022623.00599366</v>
       </c>
       <c r="G116" t="n">
-        <v>0.0000687688589096069</v>
+        <v>0</v>
       </c>
       <c r="H116" t="n">
-        <v>0.00000843405723571777</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -3517,10 +3517,10 @@
         <v>3302096.02832794</v>
       </c>
       <c r="G117" t="n">
-        <v>0.000011742115020752</v>
+        <v>0</v>
       </c>
       <c r="H117" t="n">
-        <v>0.00000974535942077637</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -3543,10 +3543,10 @@
         <v>8206689.0154779</v>
       </c>
       <c r="G118" t="n">
-        <v>0.00000357627868652344</v>
+        <v>0</v>
       </c>
       <c r="H118" t="n">
-        <v>0.000000625848770141602</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -3569,10 +3569,10 @@
         <v>4251953.9770484</v>
       </c>
       <c r="G119" t="n">
-        <v>0.00000619888305664062</v>
+        <v>0</v>
       </c>
       <c r="H119" t="n">
-        <v>0.00000298023223876953</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -3595,10 +3595,10 @@
         <v>317250.997549854</v>
       </c>
       <c r="G120" t="n">
-        <v>0.0000333786010742188</v>
+        <v>0</v>
       </c>
       <c r="H120" t="n">
-        <v>0.00000363588333129883</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -3621,10 +3621,10 @@
         <v>51653102.7579308</v>
       </c>
       <c r="G121" t="n">
-        <v>5.72513353824615</v>
+        <v>6</v>
       </c>
       <c r="H121" t="n">
-        <v>0.0000399947166442871</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -3647,10 +3647,10 @@
         <v>2430151.99910849</v>
       </c>
       <c r="G122" t="n">
-        <v>0.0000129044055938721</v>
+        <v>0</v>
       </c>
       <c r="H122" t="n">
-        <v>0.00000385940074920654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -3673,10 +3673,10 @@
         <v>15083913.783133</v>
       </c>
       <c r="G123" t="n">
-        <v>0.00000739097595214844</v>
+        <v>0</v>
       </c>
       <c r="H123" t="n">
-        <v>0.000030219554901123</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -3699,10 +3699,10 @@
         <v>4572917.03000665</v>
       </c>
       <c r="G124" t="n">
-        <v>0.00000280141830444336</v>
+        <v>0</v>
       </c>
       <c r="H124" t="n">
-        <v>0.00000631809234619141</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -3725,10 +3725,10 @@
         <v>31085397.0146179</v>
       </c>
       <c r="G125" t="n">
-        <v>0.0000321865081787109</v>
+        <v>0</v>
       </c>
       <c r="H125" t="n">
-        <v>0.00000235438346862793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -3751,10 +3751,10 @@
         <v>9116355.00341654</v>
       </c>
       <c r="G126" t="n">
-        <v>0.00000321865081787109</v>
+        <v>0</v>
       </c>
       <c r="H126" t="n">
-        <v>0.00000679492950439453</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -3777,10 +3777,10 @@
         <v>5682811.0575676</v>
       </c>
       <c r="G127" t="n">
-        <v>0.0000238418579101562</v>
+        <v>0</v>
       </c>
       <c r="H127" t="n">
-        <v>0.0000128448009490967</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -3803,10 +3803,10 @@
         <v>8692463.0048871</v>
       </c>
       <c r="G128" t="n">
-        <v>0.0000123381614685059</v>
+        <v>0</v>
       </c>
       <c r="H128" t="n">
-        <v>0.00000306963920593262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -3832,7 +3832,7 @@
         <v>0</v>
       </c>
       <c r="H129" t="n">
-        <v>0.000000178813934326172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -3855,10 +3855,10 @@
         <v>4555339.98873085</v>
       </c>
       <c r="G130" t="n">
-        <v>0.00000609457492828369</v>
+        <v>0</v>
       </c>
       <c r="H130" t="n">
-        <v>0.00000521913170814514</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
R11 ed3.0 and formatting code with Air
</commit_message>
<xml_diff>
--- a/tables/tab_weight_sums.xlsx
+++ b/tables/tab_weight_sums.xlsx
@@ -3297,19 +3297,19 @@
         <v>46</v>
       </c>
       <c r="B109" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C109" t="n">
-        <v>1384</v>
+        <v>2239</v>
       </c>
       <c r="D109" t="n">
-        <v>1384</v>
+        <v>2238.99997510016</v>
       </c>
       <c r="E109" t="n">
-        <v>1384.00001186132</v>
+        <v>2239.00000280142</v>
       </c>
       <c r="F109" t="n">
-        <v>7488624.02200699</v>
+        <v>5534290.98106921</v>
       </c>
       <c r="G109" t="n">
         <v>0</v>
@@ -3323,19 +3323,19 @@
         <v>46</v>
       </c>
       <c r="B110" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C110" t="n">
-        <v>685</v>
+        <v>1384</v>
       </c>
       <c r="D110" t="n">
-        <v>685.000018030405</v>
+        <v>1384</v>
       </c>
       <c r="E110" t="n">
-        <v>685.000001549721</v>
+        <v>1384.00001186132</v>
       </c>
       <c r="F110" t="n">
-        <v>772474.000267684</v>
+        <v>7488624.02200699</v>
       </c>
       <c r="G110" t="n">
         <v>0</v>
@@ -3349,19 +3349,19 @@
         <v>46</v>
       </c>
       <c r="B111" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C111" t="n">
-        <v>1805</v>
+        <v>685</v>
       </c>
       <c r="D111" t="n">
-        <v>1805.0000166595</v>
+        <v>685.000018030405</v>
       </c>
       <c r="E111" t="n">
-        <v>1804.99993595481</v>
+        <v>685.000001549721</v>
       </c>
       <c r="F111" t="n">
-        <v>9081752.12676031</v>
+        <v>772474.000267684</v>
       </c>
       <c r="G111" t="n">
         <v>0</v>
@@ -3375,19 +3375,19 @@
         <v>46</v>
       </c>
       <c r="B112" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C112" t="n">
-        <v>2420</v>
+        <v>1805</v>
       </c>
       <c r="D112" t="n">
-        <v>2419.99993860722</v>
+        <v>1805.0000166595</v>
       </c>
       <c r="E112" t="n">
-        <v>2419.99996938556</v>
+        <v>1804.99993595481</v>
       </c>
       <c r="F112" t="n">
-        <v>72429867.4458265</v>
+        <v>9081752.12676031</v>
       </c>
       <c r="G112" t="n">
         <v>0</v>
@@ -3401,19 +3401,19 @@
         <v>46</v>
       </c>
       <c r="B113" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C113" t="n">
-        <v>1844</v>
+        <v>2420</v>
       </c>
       <c r="D113" t="n">
-        <v>1844.00003373623</v>
+        <v>2419.99993860722</v>
       </c>
       <c r="E113" t="n">
-        <v>1843.99996042252</v>
+        <v>2419.99996938556</v>
       </c>
       <c r="F113" t="n">
-        <v>41548145.1189518</v>
+        <v>72429867.4458265</v>
       </c>
       <c r="G113" t="n">
         <v>0</v>
@@ -3427,19 +3427,19 @@
         <v>46</v>
       </c>
       <c r="B114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C114" t="n">
-        <v>1563</v>
+        <v>1844</v>
       </c>
       <c r="D114" t="n">
-        <v>1563</v>
+        <v>1844.00003373623</v>
       </c>
       <c r="E114" t="n">
-        <v>1562.99999660254</v>
+        <v>1843.99996042252</v>
       </c>
       <c r="F114" t="n">
-        <v>4723642.00651646</v>
+        <v>41548145.1189518</v>
       </c>
       <c r="G114" t="n">
         <v>0</v>
@@ -3453,19 +3453,19 @@
         <v>46</v>
       </c>
       <c r="B115" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C115" t="n">
-        <v>1771</v>
+        <v>1563</v>
       </c>
       <c r="D115" t="n">
-        <v>1770.98797518015</v>
+        <v>1563</v>
       </c>
       <c r="E115" t="n">
-        <v>1770.99999552965</v>
+        <v>1562.99999660254</v>
       </c>
       <c r="F115" t="n">
-        <v>56395314.7733212</v>
+        <v>4723642.00651646</v>
       </c>
       <c r="G115" t="n">
         <v>0</v>
@@ -3479,19 +3479,19 @@
         <v>46</v>
       </c>
       <c r="B116" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C116" t="n">
-        <v>1684</v>
+        <v>1771</v>
       </c>
       <c r="D116" t="n">
-        <v>1683.99995458126</v>
+        <v>1770.98797518015</v>
       </c>
       <c r="E116" t="n">
-        <v>1684.00000494719</v>
+        <v>1770.99999552965</v>
       </c>
       <c r="F116" t="n">
-        <v>55980686.1269474</v>
+        <v>56395314.7733212</v>
       </c>
       <c r="G116" t="n">
         <v>0</v>
@@ -3505,19 +3505,19 @@
         <v>46</v>
       </c>
       <c r="B117" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C117" t="n">
-        <v>2757</v>
+        <v>1684</v>
       </c>
       <c r="D117" t="n">
-        <v>2757.00006876886</v>
+        <v>1683.99995458126</v>
       </c>
       <c r="E117" t="n">
-        <v>2757.00000843406</v>
+        <v>1684.00000494719</v>
       </c>
       <c r="F117" t="n">
-        <v>9022623.00599366</v>
+        <v>55980686.1269474</v>
       </c>
       <c r="G117" t="n">
         <v>0</v>
@@ -3531,19 +3531,19 @@
         <v>46</v>
       </c>
       <c r="B118" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C118" t="n">
-        <v>1563</v>
+        <v>2757</v>
       </c>
       <c r="D118" t="n">
-        <v>1562.99998825788</v>
+        <v>2757.00006876886</v>
       </c>
       <c r="E118" t="n">
-        <v>1563.00000974536</v>
+        <v>2757.00000843406</v>
       </c>
       <c r="F118" t="n">
-        <v>3302096.02832794</v>
+        <v>9022623.00599366</v>
       </c>
       <c r="G118" t="n">
         <v>0</v>
@@ -3557,19 +3557,19 @@
         <v>46</v>
       </c>
       <c r="B119" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C119" t="n">
-        <v>2118</v>
+        <v>1563</v>
       </c>
       <c r="D119" t="n">
-        <v>2117.99999642372</v>
+        <v>1562.99998825788</v>
       </c>
       <c r="E119" t="n">
-        <v>2117.99999937415</v>
+        <v>1563.00000974536</v>
       </c>
       <c r="F119" t="n">
-        <v>8206689.0154779</v>
+        <v>3302096.02832794</v>
       </c>
       <c r="G119" t="n">
         <v>0</v>
@@ -3583,19 +3583,19 @@
         <v>46</v>
       </c>
       <c r="B120" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C120" t="n">
-        <v>2017</v>
+        <v>2118</v>
       </c>
       <c r="D120" t="n">
-        <v>2016.99999380112</v>
+        <v>2117.99999642372</v>
       </c>
       <c r="E120" t="n">
-        <v>2017.00000298023</v>
+        <v>2117.99999937415</v>
       </c>
       <c r="F120" t="n">
-        <v>4251953.9770484</v>
+        <v>8206689.0154779</v>
       </c>
       <c r="G120" t="n">
         <v>0</v>
@@ -3609,19 +3609,19 @@
         <v>46</v>
       </c>
       <c r="B121" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C121" t="n">
-        <v>842</v>
+        <v>2017</v>
       </c>
       <c r="D121" t="n">
-        <v>841.999966621399</v>
+        <v>2016.99999380112</v>
       </c>
       <c r="E121" t="n">
-        <v>841.999996364117</v>
+        <v>2017.00000298023</v>
       </c>
       <c r="F121" t="n">
-        <v>317250.997549854</v>
+        <v>4251953.9770484</v>
       </c>
       <c r="G121" t="n">
         <v>0</v>
@@ -3635,22 +3635,22 @@
         <v>46</v>
       </c>
       <c r="B122" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C122" t="n">
-        <v>2865</v>
+        <v>906</v>
       </c>
       <c r="D122" t="n">
-        <v>2870.72513353825</v>
+        <v>905.999990701675</v>
       </c>
       <c r="E122" t="n">
-        <v>2865.00003999472</v>
+        <v>905.999990582466</v>
       </c>
       <c r="F122" t="n">
-        <v>51653102.7579308</v>
+        <v>6750299.96842146</v>
       </c>
       <c r="G122" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -3661,19 +3661,19 @@
         <v>46</v>
       </c>
       <c r="B123" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C123" t="n">
-        <v>1365</v>
+        <v>842</v>
       </c>
       <c r="D123" t="n">
-        <v>1365.00001290441</v>
+        <v>841.999966621399</v>
       </c>
       <c r="E123" t="n">
-        <v>1364.9999961406</v>
+        <v>841.999996364117</v>
       </c>
       <c r="F123" t="n">
-        <v>2430151.99910849</v>
+        <v>317250.997549854</v>
       </c>
       <c r="G123" t="n">
         <v>0</v>
@@ -3687,22 +3687,22 @@
         <v>46</v>
       </c>
       <c r="B124" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C124" t="n">
-        <v>1695</v>
+        <v>2865</v>
       </c>
       <c r="D124" t="n">
-        <v>1695.00000739098</v>
+        <v>2870.72513353825</v>
       </c>
       <c r="E124" t="n">
-        <v>1694.99996978045</v>
+        <v>2865.00003999472</v>
       </c>
       <c r="F124" t="n">
-        <v>15083913.783133</v>
+        <v>51653102.7579308</v>
       </c>
       <c r="G124" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -3713,19 +3713,19 @@
         <v>46</v>
       </c>
       <c r="B125" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C125" t="n">
-        <v>1337</v>
+        <v>1365</v>
       </c>
       <c r="D125" t="n">
-        <v>1336.99999719858</v>
+        <v>1365.00001290441</v>
       </c>
       <c r="E125" t="n">
-        <v>1337.00000631809</v>
+        <v>1364.9999961406</v>
       </c>
       <c r="F125" t="n">
-        <v>4572917.03000665</v>
+        <v>2430151.99910849</v>
       </c>
       <c r="G125" t="n">
         <v>0</v>
@@ -3739,19 +3739,19 @@
         <v>46</v>
       </c>
       <c r="B126" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C126" t="n">
-        <v>1442</v>
+        <v>1252</v>
       </c>
       <c r="D126" t="n">
-        <v>1441.99996781349</v>
+        <v>1252.00000301003</v>
       </c>
       <c r="E126" t="n">
-        <v>1442.00000235438</v>
+        <v>1252.00000101328</v>
       </c>
       <c r="F126" t="n">
-        <v>31085397.0146179</v>
+        <v>1582531.00175411</v>
       </c>
       <c r="G126" t="n">
         <v>0</v>
@@ -3765,19 +3765,19 @@
         <v>46</v>
       </c>
       <c r="B127" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C127" t="n">
-        <v>1373</v>
+        <v>1609</v>
       </c>
       <c r="D127" t="n">
-        <v>1373.00000321865</v>
+        <v>1609.0000321418</v>
       </c>
       <c r="E127" t="n">
-        <v>1373.00000679493</v>
+        <v>1609.00002001971</v>
       </c>
       <c r="F127" t="n">
-        <v>9116355.00341654</v>
+        <v>506465.000677854</v>
       </c>
       <c r="G127" t="n">
         <v>0</v>
@@ -3791,19 +3791,19 @@
         <v>46</v>
       </c>
       <c r="B128" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C128" t="n">
-        <v>1563</v>
+        <v>1695</v>
       </c>
       <c r="D128" t="n">
-        <v>1563.00002384186</v>
+        <v>1695.00000739098</v>
       </c>
       <c r="E128" t="n">
-        <v>1563.0000128448</v>
+        <v>1694.99996978045</v>
       </c>
       <c r="F128" t="n">
-        <v>5682811.0575676</v>
+        <v>15083913.783133</v>
       </c>
       <c r="G128" t="n">
         <v>0</v>
@@ -3817,19 +3817,19 @@
         <v>46</v>
       </c>
       <c r="B129" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C129" t="n">
-        <v>1230</v>
+        <v>1337</v>
       </c>
       <c r="D129" t="n">
-        <v>1229.99998766184</v>
+        <v>1336.99999719858</v>
       </c>
       <c r="E129" t="n">
-        <v>1230.00000306964</v>
+        <v>1337.00000631809</v>
       </c>
       <c r="F129" t="n">
-        <v>8692463.0048871</v>
+        <v>4572917.03000665</v>
       </c>
       <c r="G129" t="n">
         <v>0</v>
@@ -3843,19 +3843,19 @@
         <v>46</v>
       </c>
       <c r="B130" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C130" t="n">
-        <v>1248</v>
+        <v>1442</v>
       </c>
       <c r="D130" t="n">
-        <v>1248</v>
+        <v>1441.99996781349</v>
       </c>
       <c r="E130" t="n">
-        <v>1248.00000017881</v>
+        <v>1442.00000235438</v>
       </c>
       <c r="F130" t="n">
-        <v>1799440.98971784</v>
+        <v>31085397.0146179</v>
       </c>
       <c r="G130" t="n">
         <v>0</v>
@@ -3869,24 +3869,128 @@
         <v>46</v>
       </c>
       <c r="B131" t="s">
+        <v>27</v>
+      </c>
+      <c r="C131" t="n">
+        <v>1373</v>
+      </c>
+      <c r="D131" t="n">
+        <v>1373.00000321865</v>
+      </c>
+      <c r="E131" t="n">
+        <v>1373.00000679493</v>
+      </c>
+      <c r="F131" t="n">
+        <v>9116355.00341654</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>46</v>
+      </c>
+      <c r="B132" t="s">
+        <v>40</v>
+      </c>
+      <c r="C132" t="n">
+        <v>1563</v>
+      </c>
+      <c r="D132" t="n">
+        <v>1563.00002384186</v>
+      </c>
+      <c r="E132" t="n">
+        <v>1563.0000128448</v>
+      </c>
+      <c r="F132" t="n">
+        <v>5682811.0575676</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>46</v>
+      </c>
+      <c r="B133" t="s">
+        <v>28</v>
+      </c>
+      <c r="C133" t="n">
+        <v>1230</v>
+      </c>
+      <c r="D133" t="n">
+        <v>1229.99998766184</v>
+      </c>
+      <c r="E133" t="n">
+        <v>1230.00000306964</v>
+      </c>
+      <c r="F133" t="n">
+        <v>8692463.0048871</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>46</v>
+      </c>
+      <c r="B134" t="s">
+        <v>29</v>
+      </c>
+      <c r="C134" t="n">
+        <v>1248</v>
+      </c>
+      <c r="D134" t="n">
+        <v>1248</v>
+      </c>
+      <c r="E134" t="n">
+        <v>1248.00000017881</v>
+      </c>
+      <c r="F134" t="n">
+        <v>1799440.98971784</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0</v>
+      </c>
+      <c r="H134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>46</v>
+      </c>
+      <c r="B135" t="s">
         <v>41</v>
       </c>
-      <c r="C131" t="n">
+      <c r="C135" t="n">
         <v>1442</v>
       </c>
-      <c r="D131" t="n">
+      <c r="D135" t="n">
         <v>1442.00000609457</v>
       </c>
-      <c r="E131" t="n">
+      <c r="E135" t="n">
         <v>1441.99999478087</v>
       </c>
-      <c r="F131" t="n">
+      <c r="F135" t="n">
         <v>4555339.98873085</v>
       </c>
-      <c r="G131" t="n">
-        <v>0</v>
-      </c>
-      <c r="H131" t="n">
+      <c r="G135" t="n">
+        <v>0</v>
+      </c>
+      <c r="H135" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ESS11 edition 4.0: add install script & new data, update .Rprofile, parsing, validation, tables/variables and plots; remove old install and project file.
</commit_message>
<xml_diff>
--- a/tables/tab_weight_sums.xlsx
+++ b/tables/tab_weight_sums.xlsx
@@ -3427,19 +3427,19 @@
         <v>46</v>
       </c>
       <c r="B114" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C114" t="n">
-        <v>1844</v>
+        <v>1293</v>
       </c>
       <c r="D114" t="n">
-        <v>1844.00003373623</v>
+        <v>1292.99997454882</v>
       </c>
       <c r="E114" t="n">
-        <v>1843.99996042252</v>
+        <v>1292.99996763468</v>
       </c>
       <c r="F114" t="n">
-        <v>41548145.1189518</v>
+        <v>1141964.9771601</v>
       </c>
       <c r="G114" t="n">
         <v>0</v>
@@ -3453,19 +3453,19 @@
         <v>46</v>
       </c>
       <c r="B115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C115" t="n">
-        <v>1563</v>
+        <v>1844</v>
       </c>
       <c r="D115" t="n">
-        <v>1563</v>
+        <v>1844.00003373623</v>
       </c>
       <c r="E115" t="n">
-        <v>1562.99999660254</v>
+        <v>1843.99996042252</v>
       </c>
       <c r="F115" t="n">
-        <v>4723642.00651646</v>
+        <v>41548145.1189518</v>
       </c>
       <c r="G115" t="n">
         <v>0</v>
@@ -3479,19 +3479,19 @@
         <v>46</v>
       </c>
       <c r="B116" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C116" t="n">
-        <v>1771</v>
+        <v>1563</v>
       </c>
       <c r="D116" t="n">
-        <v>1770.98797518015</v>
+        <v>1563</v>
       </c>
       <c r="E116" t="n">
-        <v>1770.99999552965</v>
+        <v>1562.99999660254</v>
       </c>
       <c r="F116" t="n">
-        <v>56395314.7733212</v>
+        <v>4723642.00651646</v>
       </c>
       <c r="G116" t="n">
         <v>0</v>
@@ -3505,19 +3505,19 @@
         <v>46</v>
       </c>
       <c r="B117" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C117" t="n">
-        <v>1684</v>
+        <v>1771</v>
       </c>
       <c r="D117" t="n">
-        <v>1683.99995458126</v>
+        <v>1770.98797518015</v>
       </c>
       <c r="E117" t="n">
-        <v>1684.00000494719</v>
+        <v>1770.99999552965</v>
       </c>
       <c r="F117" t="n">
-        <v>55980686.1269474</v>
+        <v>56395314.7733212</v>
       </c>
       <c r="G117" t="n">
         <v>0</v>
@@ -3531,19 +3531,19 @@
         <v>46</v>
       </c>
       <c r="B118" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C118" t="n">
-        <v>2757</v>
+        <v>1684</v>
       </c>
       <c r="D118" t="n">
-        <v>2757.00006876886</v>
+        <v>1683.99995458126</v>
       </c>
       <c r="E118" t="n">
-        <v>2757.00000843406</v>
+        <v>1684.00000494719</v>
       </c>
       <c r="F118" t="n">
-        <v>9022623.00599366</v>
+        <v>55980686.1269474</v>
       </c>
       <c r="G118" t="n">
         <v>0</v>
@@ -3557,19 +3557,19 @@
         <v>46</v>
       </c>
       <c r="B119" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C119" t="n">
-        <v>1563</v>
+        <v>2757</v>
       </c>
       <c r="D119" t="n">
-        <v>1562.99998825788</v>
+        <v>2757.00006876886</v>
       </c>
       <c r="E119" t="n">
-        <v>1563.00000974536</v>
+        <v>2757.00000843406</v>
       </c>
       <c r="F119" t="n">
-        <v>3302096.02832794</v>
+        <v>9022623.00599366</v>
       </c>
       <c r="G119" t="n">
         <v>0</v>
@@ -3583,19 +3583,19 @@
         <v>46</v>
       </c>
       <c r="B120" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C120" t="n">
-        <v>2118</v>
+        <v>1563</v>
       </c>
       <c r="D120" t="n">
-        <v>2117.99999642372</v>
+        <v>1562.99998825788</v>
       </c>
       <c r="E120" t="n">
-        <v>2117.99999937415</v>
+        <v>1563.00000974536</v>
       </c>
       <c r="F120" t="n">
-        <v>8206689.0154779</v>
+        <v>3302096.02832794</v>
       </c>
       <c r="G120" t="n">
         <v>0</v>
@@ -3609,19 +3609,19 @@
         <v>46</v>
       </c>
       <c r="B121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C121" t="n">
-        <v>2017</v>
+        <v>2118</v>
       </c>
       <c r="D121" t="n">
-        <v>2016.99999380112</v>
+        <v>2117.99999642372</v>
       </c>
       <c r="E121" t="n">
-        <v>2017.00000298023</v>
+        <v>2117.99999937415</v>
       </c>
       <c r="F121" t="n">
-        <v>4251953.9770484</v>
+        <v>8206689.0154779</v>
       </c>
       <c r="G121" t="n">
         <v>0</v>
@@ -3635,19 +3635,19 @@
         <v>46</v>
       </c>
       <c r="B122" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C122" t="n">
-        <v>906</v>
+        <v>2017</v>
       </c>
       <c r="D122" t="n">
-        <v>905.999990701675</v>
+        <v>2016.99999380112</v>
       </c>
       <c r="E122" t="n">
-        <v>905.999990582466</v>
+        <v>2017.00000298023</v>
       </c>
       <c r="F122" t="n">
-        <v>6750299.96842146</v>
+        <v>4251953.9770484</v>
       </c>
       <c r="G122" t="n">
         <v>0</v>
@@ -3661,19 +3661,19 @@
         <v>46</v>
       </c>
       <c r="B123" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C123" t="n">
-        <v>842</v>
+        <v>906</v>
       </c>
       <c r="D123" t="n">
-        <v>841.999966621399</v>
+        <v>905.999990701675</v>
       </c>
       <c r="E123" t="n">
-        <v>841.999996364117</v>
+        <v>905.999990582466</v>
       </c>
       <c r="F123" t="n">
-        <v>317250.997549854</v>
+        <v>6750299.96842146</v>
       </c>
       <c r="G123" t="n">
         <v>0</v>
@@ -3687,22 +3687,22 @@
         <v>46</v>
       </c>
       <c r="B124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C124" t="n">
-        <v>2865</v>
+        <v>842</v>
       </c>
       <c r="D124" t="n">
-        <v>2870.72513353825</v>
+        <v>841.999966621399</v>
       </c>
       <c r="E124" t="n">
-        <v>2865.00003999472</v>
+        <v>841.999996364117</v>
       </c>
       <c r="F124" t="n">
-        <v>51653102.7579308</v>
+        <v>317250.997549854</v>
       </c>
       <c r="G124" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -3713,22 +3713,22 @@
         <v>46</v>
       </c>
       <c r="B125" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C125" t="n">
-        <v>1365</v>
+        <v>2865</v>
       </c>
       <c r="D125" t="n">
-        <v>1365.00001290441</v>
+        <v>2870.72513353825</v>
       </c>
       <c r="E125" t="n">
-        <v>1364.9999961406</v>
+        <v>2865.00003999472</v>
       </c>
       <c r="F125" t="n">
-        <v>2430151.99910849</v>
+        <v>51653102.7579308</v>
       </c>
       <c r="G125" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -3739,19 +3739,19 @@
         <v>46</v>
       </c>
       <c r="B126" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C126" t="n">
-        <v>1252</v>
+        <v>1365</v>
       </c>
       <c r="D126" t="n">
-        <v>1252.00000301003</v>
+        <v>1365.00001290441</v>
       </c>
       <c r="E126" t="n">
-        <v>1252.00000101328</v>
+        <v>1364.9999961406</v>
       </c>
       <c r="F126" t="n">
-        <v>1582531.00175411</v>
+        <v>2430151.99910849</v>
       </c>
       <c r="G126" t="n">
         <v>0</v>
@@ -3765,19 +3765,19 @@
         <v>46</v>
       </c>
       <c r="B127" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C127" t="n">
-        <v>1609</v>
+        <v>1252</v>
       </c>
       <c r="D127" t="n">
-        <v>1609.0000321418</v>
+        <v>1252.00000301003</v>
       </c>
       <c r="E127" t="n">
-        <v>1609.00002001971</v>
+        <v>1252.00000101328</v>
       </c>
       <c r="F127" t="n">
-        <v>506465.000677854</v>
+        <v>1582531.00175411</v>
       </c>
       <c r="G127" t="n">
         <v>0</v>
@@ -3791,19 +3791,19 @@
         <v>46</v>
       </c>
       <c r="B128" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C128" t="n">
-        <v>1695</v>
+        <v>1609</v>
       </c>
       <c r="D128" t="n">
-        <v>1695.00000739098</v>
+        <v>1609.0000321418</v>
       </c>
       <c r="E128" t="n">
-        <v>1694.99996978045</v>
+        <v>1609.00002001971</v>
       </c>
       <c r="F128" t="n">
-        <v>15083913.783133</v>
+        <v>506465.000677854</v>
       </c>
       <c r="G128" t="n">
         <v>0</v>
@@ -3817,19 +3817,19 @@
         <v>46</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C129" t="n">
-        <v>1337</v>
+        <v>1695</v>
       </c>
       <c r="D129" t="n">
-        <v>1336.99999719858</v>
+        <v>1695.00000739098</v>
       </c>
       <c r="E129" t="n">
-        <v>1337.00000631809</v>
+        <v>1694.99996978045</v>
       </c>
       <c r="F129" t="n">
-        <v>4572917.03000665</v>
+        <v>15083913.783133</v>
       </c>
       <c r="G129" t="n">
         <v>0</v>
@@ -3843,19 +3843,19 @@
         <v>46</v>
       </c>
       <c r="B130" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C130" t="n">
-        <v>1442</v>
+        <v>1337</v>
       </c>
       <c r="D130" t="n">
-        <v>1441.99996781349</v>
+        <v>1336.99999719858</v>
       </c>
       <c r="E130" t="n">
-        <v>1442.00000235438</v>
+        <v>1337.00000631809</v>
       </c>
       <c r="F130" t="n">
-        <v>31085397.0146179</v>
+        <v>4572917.03000665</v>
       </c>
       <c r="G130" t="n">
         <v>0</v>
@@ -3869,19 +3869,19 @@
         <v>46</v>
       </c>
       <c r="B131" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C131" t="n">
-        <v>1373</v>
+        <v>1442</v>
       </c>
       <c r="D131" t="n">
-        <v>1373.00000321865</v>
+        <v>1441.99996781349</v>
       </c>
       <c r="E131" t="n">
-        <v>1373.00000679493</v>
+        <v>1442.00000235438</v>
       </c>
       <c r="F131" t="n">
-        <v>9116355.00341654</v>
+        <v>31085397.0146179</v>
       </c>
       <c r="G131" t="n">
         <v>0</v>
@@ -3895,19 +3895,19 @@
         <v>46</v>
       </c>
       <c r="B132" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C132" t="n">
-        <v>1563</v>
+        <v>1373</v>
       </c>
       <c r="D132" t="n">
-        <v>1563.00002384186</v>
+        <v>1373.00000321865</v>
       </c>
       <c r="E132" t="n">
-        <v>1563.0000128448</v>
+        <v>1373.00000679493</v>
       </c>
       <c r="F132" t="n">
-        <v>5682811.0575676</v>
+        <v>9116355.00341654</v>
       </c>
       <c r="G132" t="n">
         <v>0</v>
@@ -3921,19 +3921,19 @@
         <v>46</v>
       </c>
       <c r="B133" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C133" t="n">
-        <v>1230</v>
+        <v>1563</v>
       </c>
       <c r="D133" t="n">
-        <v>1229.99998766184</v>
+        <v>1563.00002384186</v>
       </c>
       <c r="E133" t="n">
-        <v>1230.00000306964</v>
+        <v>1563.0000128448</v>
       </c>
       <c r="F133" t="n">
-        <v>8692463.0048871</v>
+        <v>5682811.0575676</v>
       </c>
       <c r="G133" t="n">
         <v>0</v>
@@ -3947,19 +3947,19 @@
         <v>46</v>
       </c>
       <c r="B134" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C134" t="n">
-        <v>1248</v>
+        <v>1230</v>
       </c>
       <c r="D134" t="n">
-        <v>1248</v>
+        <v>1229.99998766184</v>
       </c>
       <c r="E134" t="n">
-        <v>1248.00000017881</v>
+        <v>1230.00000306964</v>
       </c>
       <c r="F134" t="n">
-        <v>1799440.98971784</v>
+        <v>8692463.0048871</v>
       </c>
       <c r="G134" t="n">
         <v>0</v>
@@ -3973,24 +3973,76 @@
         <v>46</v>
       </c>
       <c r="B135" t="s">
+        <v>29</v>
+      </c>
+      <c r="C135" t="n">
+        <v>1248</v>
+      </c>
+      <c r="D135" t="n">
+        <v>1248</v>
+      </c>
+      <c r="E135" t="n">
+        <v>1248.00000017881</v>
+      </c>
+      <c r="F135" t="n">
+        <v>1799440.98971784</v>
+      </c>
+      <c r="G135" t="n">
+        <v>0</v>
+      </c>
+      <c r="H135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>46</v>
+      </c>
+      <c r="B136" t="s">
         <v>41</v>
       </c>
-      <c r="C135" t="n">
+      <c r="C136" t="n">
         <v>1442</v>
       </c>
-      <c r="D135" t="n">
+      <c r="D136" t="n">
         <v>1442.00000609457</v>
       </c>
-      <c r="E135" t="n">
+      <c r="E136" t="n">
         <v>1441.99999478087</v>
       </c>
-      <c r="F135" t="n">
+      <c r="F136" t="n">
         <v>4555339.98873085</v>
       </c>
-      <c r="G135" t="n">
-        <v>0</v>
-      </c>
-      <c r="H135" t="n">
+      <c r="G136" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>46</v>
+      </c>
+      <c r="B137" t="s">
+        <v>45</v>
+      </c>
+      <c r="C137" t="n">
+        <v>2661</v>
+      </c>
+      <c r="D137" t="n">
+        <v>2661.00006902218</v>
+      </c>
+      <c r="E137" t="n">
+        <v>2661.00006902218</v>
+      </c>
+      <c r="F137" t="n">
+        <v>34877812.7890825</v>
+      </c>
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>